<commit_message>
master table over 1K hits limit; Site_Ind_Skel updated with new template
</commit_message>
<xml_diff>
--- a/UploadData/Site_Ind_Skel/Template_Site_Skel_Ind.xlsx
+++ b/UploadData/Site_Ind_Skel/Template_Site_Skel_Ind.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrespc/Documents/PostDocPasteur/aDNA/Import_eLAB/API_FUNCTIONALITIES/UploadData/Site_Ind_Skel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788430D8-7C8E-124A-AAAA-C143E7B9583A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DD7ABB-ECC1-D64F-ADA6-6C87D5E5B032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16680" xr2:uid="{5E5F3F6A-7BA4-074F-8F96-23DEB4E79118}"/>
   </bookViews>
@@ -34,78 +34,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>Site_Main geographic region</t>
-  </si>
-  <si>
-    <t>Site_Country</t>
-  </si>
-  <si>
-    <t>Site_Province / Region</t>
-  </si>
-  <si>
-    <t>Site_Locality</t>
-  </si>
-  <si>
-    <t>Site_Latitude</t>
-  </si>
-  <si>
-    <t>Site_Longitude</t>
-  </si>
-  <si>
-    <t>Site_Site type</t>
-  </si>
-  <si>
-    <t>Individual_Archaeologist Observations</t>
-  </si>
-  <si>
-    <t>Individual_Archaeologist ID</t>
-  </si>
-  <si>
-    <t>Individual_Archaeologist group</t>
-  </si>
-  <si>
-    <t>Individual_Date</t>
-  </si>
-  <si>
-    <t>Individual_Datation method</t>
-  </si>
-  <si>
-    <t>Individual_Subsistence Strategy</t>
-  </si>
-  <si>
-    <t>Individual_Age</t>
-  </si>
-  <si>
-    <t>Individual_Gender</t>
-  </si>
-  <si>
-    <t>Skeleton Element_Archaeologist sample ID</t>
-  </si>
-  <si>
-    <t>Skeleton Element_description</t>
-  </si>
-  <si>
-    <t>Skeleton Element_Pictures Labelling</t>
-  </si>
-  <si>
-    <t>Skeleton Element_Skeleton element</t>
-  </si>
-  <si>
-    <t>Skeleton Element_Exportation Permit Number</t>
-  </si>
-  <si>
-    <t>Skeleton Element_Observation Labelling</t>
-  </si>
-  <si>
-    <t>Skeleton Element_Observation Scanning</t>
-  </si>
-  <si>
-    <t>Skeleton Element_Scanned</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t>INFORMATION FOR ARCHAEOLOGICAL SITE</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Province / Region</t>
+  </si>
+  <si>
+    <t>Locality</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Site type</t>
+  </si>
+  <si>
+    <t>Archaeologist ID</t>
+  </si>
+  <si>
+    <t>Archaeologist group</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Datation method</t>
+  </si>
+  <si>
+    <t>Subsistence Strategy</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Archaeologist Observations</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Pictures Labelling</t>
+  </si>
+  <si>
+    <t>Skeleton element</t>
+  </si>
+  <si>
+    <t>Exportation Permit Number</t>
+  </si>
+  <si>
+    <t>Observation Labelling</t>
+  </si>
+  <si>
+    <t>Scanned</t>
+  </si>
+  <si>
+    <t>Observation Scanning</t>
+  </si>
+  <si>
+    <t>INFORMATION FOR INDIVIDUAL</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Main Geographic Region</t>
+  </si>
+  <si>
+    <t>RascovanLab ID</t>
+  </si>
+  <si>
+    <t>INFORMATION FOR SKELETON ELEMENT</t>
   </si>
 </sst>
 </file>
@@ -121,15 +130,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -137,18 +164,226 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3000"/>
+      <color rgb="FFFE4E65"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -457,107 +692,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2196C8FF-DBEE-7842-AE12-2E595FBCD423}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" style="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.83203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24" style="26" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" style="26" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" style="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:24" s="6" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+    </row>
+    <row r="2" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X2" s="22" t="s">
         <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:Q1"/>
+    <mergeCell ref="R1:X1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>